<commit_message>
Phase 11 - Onglet 3 Amortissements: Isolation complète avec property_id
- Backend: 13 endpoints modifiés avec property_id (9 amortization_types + 4 amortization)
- Frontend: AmortizationTable et AmortizationConfigCard utilisent activeProperty.id
- Tests: Isolation backend/frontend + non-régression (15 tests)
- Migration: Scripts de migration et validation créés
- Correction régression: /transactions/unique-values filtre maintenant par property_id
- Correction bug mapping: Seuil de similarité 70% pour éviter mappings génériques
- Mappings hardcodés: Mis à jour depuis mappings_obligatoires.xlsx (56 mappings)
</commit_message>
<xml_diff>
--- a/scripts/mappings_obligatoires.xlsx
+++ b/scripts/mappings_obligatoires.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisgarnier/Library/Mobile Documents/com~apple~CloudDocs/Python/DEV/LMNP/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisgarnier/Desktop/LMNP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889DB4C7-0717-5C46-A8C7-D3D716149E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FB1DA0-BCDF-1048-A2BA-3321BABE213D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8840" yWindow="-18680" windowWidth="27240" windowHeight="16440" xr2:uid="{3C58CE6F-3376-0749-B7FC-62A33F156F1D}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$52</definedName>
   </definedNames>
-  <calcPr calcId="181029" calcOnSave="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="77">
   <si>
     <t>Level 1</t>
   </si>
@@ -258,29 +258,28 @@
   </si>
   <si>
     <t>Service bancaires et assimile</t>
+  </si>
+  <si>
+    <t>Immobilisation Facade/Toiture</t>
+  </si>
+  <si>
+    <t>Immobilisation IGT</t>
+  </si>
+  <si>
+    <t>Immobilisation agencements</t>
+  </si>
+  <si>
+    <t>Immobilisation structure/GO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -306,10 +305,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5723BEB6-E82D-0E4A-A442-B2595EA9A82D}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,10 +652,11 @@
     <col min="1" max="1" width="64.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -669,10 +667,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2" t="s">
@@ -680,10 +678,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
       <c r="C3" t="s">
@@ -691,10 +689,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="s">
@@ -702,10 +700,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
@@ -713,10 +711,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="s">
@@ -724,10 +722,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
@@ -735,10 +733,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -746,10 +744,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>44</v>
       </c>
       <c r="C9" t="s">
@@ -757,10 +755,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>44</v>
       </c>
       <c r="C10" t="s">
@@ -768,10 +766,10 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>44</v>
       </c>
       <c r="C11" t="s">
@@ -779,10 +777,10 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>44</v>
       </c>
       <c r="C12" t="s">
@@ -790,10 +788,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>44</v>
       </c>
       <c r="C13" t="s">
@@ -801,10 +799,10 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>44</v>
       </c>
       <c r="C14" t="s">
@@ -812,10 +810,10 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" t="s">
@@ -823,10 +821,10 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
@@ -834,10 +832,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>34</v>
       </c>
       <c r="C17" t="s">
@@ -845,10 +843,10 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>34</v>
       </c>
       <c r="C18" t="s">
@@ -856,10 +854,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>34</v>
       </c>
       <c r="C19" t="s">
@@ -867,10 +865,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
@@ -878,10 +876,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>42</v>
       </c>
       <c r="C21" t="s">
@@ -889,10 +887,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>42</v>
       </c>
       <c r="C22" t="s">
@@ -900,10 +898,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>30</v>
       </c>
       <c r="C23" t="s">
@@ -911,10 +909,10 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>30</v>
       </c>
       <c r="C24" t="s">
@@ -922,10 +920,10 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>30</v>
       </c>
       <c r="C25" t="s">
@@ -933,10 +931,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>30</v>
       </c>
       <c r="C26" t="s">
@@ -944,10 +942,10 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>4</v>
       </c>
       <c r="C27" t="s">
@@ -955,10 +953,10 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>4</v>
       </c>
       <c r="C28" t="s">
@@ -966,10 +964,10 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>4</v>
       </c>
       <c r="C29" t="s">
@@ -977,43 +975,43 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>27</v>
       </c>
       <c r="C33" t="s">
@@ -1021,10 +1019,10 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>27</v>
       </c>
       <c r="C34" t="s">
@@ -1032,10 +1030,10 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>27</v>
       </c>
       <c r="C35" t="s">
@@ -1043,10 +1041,10 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>27</v>
       </c>
       <c r="C36" t="s">
@@ -1054,10 +1052,10 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>27</v>
       </c>
       <c r="C37" t="s">
@@ -1065,10 +1063,10 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>9</v>
       </c>
       <c r="C38" t="s">
@@ -1076,10 +1074,10 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>9</v>
       </c>
       <c r="C39" t="s">
@@ -1087,10 +1085,10 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>9</v>
       </c>
       <c r="C40" t="s">
@@ -1098,7 +1096,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>64</v>
       </c>
       <c r="B41" t="s">
@@ -1109,7 +1107,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>15</v>
       </c>
       <c r="B42" t="s">
@@ -1120,7 +1118,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>65</v>
       </c>
       <c r="B43" t="s">
@@ -1131,7 +1129,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>23</v>
       </c>
       <c r="B44" t="s">
@@ -1142,7 +1140,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>66</v>
       </c>
       <c r="B45" t="s">
@@ -1153,7 +1151,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>39</v>
       </c>
       <c r="B46" t="s">
@@ -1164,7 +1162,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>37</v>
       </c>
       <c r="B47" t="s">
@@ -1175,10 +1173,10 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>11</v>
       </c>
       <c r="C48" t="s">
@@ -1186,7 +1184,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>69</v>
       </c>
       <c r="B49" t="s">
@@ -1230,14 +1228,58 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="A53" t="s">
         <v>72</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>5</v>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>73</v>
+      </c>
+      <c r="B54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>